<commit_message>
feat: Nir_GRNTI schema and GRNTI model
</commit_message>
<xml_diff>
--- a/data/grntirub.xlsx
+++ b/data/grntirub.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Programs\PyProjects\subd\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A1FC0A-A90C-4EF0-ABA2-B77FBBA7C31C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27652DDD-6AFD-45D2-9534-B2E5913D39B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -902,7 +902,7 @@
   <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:A70"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>